<commit_message>
Documents for 30% ready.
</commit_message>
<xml_diff>
--- a/docs/30%-presentation/Gantt Chart/Liver Tumor Segmentation Gantt Chart-30%.xlsx
+++ b/docs/30%-presentation/Gantt Chart/Liver Tumor Segmentation Gantt Chart-30%.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{978AEDF5-29F2-4DB1-9EA3-DA1B4F262919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97593877-78D6-43B0-BCC5-22E627798339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1905,9 +1905,9 @@
   </sheetPr>
   <dimension ref="A1:JS30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="112" zoomScaleNormal="81" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="81" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.44140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1965,11 +1965,11 @@
       </c>
       <c r="C4" s="61"/>
       <c r="D4" s="5">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G4" s="91">
         <f>G5</f>
-        <v>45747</v>
+        <v>45586</v>
       </c>
       <c r="H4" s="92"/>
       <c r="I4" s="92"/>
@@ -1979,7 +1979,7 @@
       <c r="M4" s="93"/>
       <c r="N4" s="91">
         <f>N5</f>
-        <v>45754</v>
+        <v>45593</v>
       </c>
       <c r="O4" s="92"/>
       <c r="P4" s="92"/>
@@ -1989,7 +1989,7 @@
       <c r="T4" s="93"/>
       <c r="U4" s="91">
         <f>U5</f>
-        <v>45761</v>
+        <v>45600</v>
       </c>
       <c r="V4" s="92"/>
       <c r="W4" s="92"/>
@@ -1999,7 +1999,7 @@
       <c r="AA4" s="93"/>
       <c r="AB4" s="91">
         <f>AB5</f>
-        <v>45768</v>
+        <v>45607</v>
       </c>
       <c r="AC4" s="92"/>
       <c r="AD4" s="92"/>
@@ -2009,7 +2009,7 @@
       <c r="AH4" s="93"/>
       <c r="AI4" s="91">
         <f>AI5</f>
-        <v>45775</v>
+        <v>45614</v>
       </c>
       <c r="AJ4" s="92"/>
       <c r="AK4" s="92"/>
@@ -2019,7 +2019,7 @@
       <c r="AO4" s="93"/>
       <c r="AP4" s="91">
         <f>AP5</f>
-        <v>45782</v>
+        <v>45621</v>
       </c>
       <c r="AQ4" s="92"/>
       <c r="AR4" s="92"/>
@@ -2029,7 +2029,7 @@
       <c r="AV4" s="93"/>
       <c r="AW4" s="91">
         <f>AW5</f>
-        <v>45789</v>
+        <v>45628</v>
       </c>
       <c r="AX4" s="92"/>
       <c r="AY4" s="92"/>
@@ -2039,7 +2039,7 @@
       <c r="BC4" s="93"/>
       <c r="BD4" s="91">
         <f>BD5</f>
-        <v>45796</v>
+        <v>45635</v>
       </c>
       <c r="BE4" s="92"/>
       <c r="BF4" s="92"/>
@@ -2049,7 +2049,7 @@
       <c r="BJ4" s="93"/>
       <c r="BK4" s="91">
         <f>BK5</f>
-        <v>45803</v>
+        <v>45642</v>
       </c>
       <c r="BL4" s="92"/>
       <c r="BM4" s="92"/>
@@ -2059,7 +2059,7 @@
       <c r="BQ4" s="93"/>
       <c r="BR4" s="91">
         <f>BR5</f>
-        <v>45810</v>
+        <v>45649</v>
       </c>
       <c r="BS4" s="92"/>
       <c r="BT4" s="92"/>
@@ -2069,7 +2069,7 @@
       <c r="BX4" s="93"/>
       <c r="BY4" s="91">
         <f>BY5</f>
-        <v>45817</v>
+        <v>45656</v>
       </c>
       <c r="BZ4" s="92"/>
       <c r="CA4" s="92"/>
@@ -2079,7 +2079,7 @@
       <c r="CE4" s="93"/>
       <c r="CF4" s="91">
         <f>CF5</f>
-        <v>45824</v>
+        <v>45663</v>
       </c>
       <c r="CG4" s="92"/>
       <c r="CH4" s="92"/>
@@ -2089,7 +2089,7 @@
       <c r="CL4" s="93"/>
       <c r="CM4" s="91">
         <f>CM5</f>
-        <v>45831</v>
+        <v>45670</v>
       </c>
       <c r="CN4" s="92"/>
       <c r="CO4" s="92"/>
@@ -2099,7 +2099,7 @@
       <c r="CS4" s="93"/>
       <c r="CT4" s="91">
         <f>CT5</f>
-        <v>45838</v>
+        <v>45677</v>
       </c>
       <c r="CU4" s="92"/>
       <c r="CV4" s="92"/>
@@ -2109,7 +2109,7 @@
       <c r="CZ4" s="93"/>
       <c r="DA4" s="91">
         <f>DA5</f>
-        <v>45845</v>
+        <v>45684</v>
       </c>
       <c r="DB4" s="92"/>
       <c r="DC4" s="92"/>
@@ -2119,7 +2119,7 @@
       <c r="DG4" s="93"/>
       <c r="DH4" s="91">
         <f>DH5</f>
-        <v>45852</v>
+        <v>45691</v>
       </c>
       <c r="DI4" s="92"/>
       <c r="DJ4" s="92"/>
@@ -2129,7 +2129,7 @@
       <c r="DN4" s="93"/>
       <c r="DO4" s="91">
         <f>DO5</f>
-        <v>45859</v>
+        <v>45698</v>
       </c>
       <c r="DP4" s="92"/>
       <c r="DQ4" s="92"/>
@@ -2139,7 +2139,7 @@
       <c r="DU4" s="93"/>
       <c r="DV4" s="91">
         <f>DV5</f>
-        <v>45866</v>
+        <v>45705</v>
       </c>
       <c r="DW4" s="92"/>
       <c r="DX4" s="92"/>
@@ -2149,7 +2149,7 @@
       <c r="EB4" s="93"/>
       <c r="EC4" s="91">
         <f>EC5</f>
-        <v>45873</v>
+        <v>45712</v>
       </c>
       <c r="ED4" s="92"/>
       <c r="EE4" s="92"/>
@@ -2159,7 +2159,7 @@
       <c r="EI4" s="93"/>
       <c r="EJ4" s="91">
         <f>EJ5</f>
-        <v>45880</v>
+        <v>45719</v>
       </c>
       <c r="EK4" s="92"/>
       <c r="EL4" s="92"/>
@@ -2169,7 +2169,7 @@
       <c r="EP4" s="93"/>
       <c r="EQ4" s="91">
         <f>EQ5</f>
-        <v>45887</v>
+        <v>45726</v>
       </c>
       <c r="ER4" s="92"/>
       <c r="ES4" s="92"/>
@@ -2179,7 +2179,7 @@
       <c r="EW4" s="93"/>
       <c r="EX4" s="91">
         <f>EX5</f>
-        <v>45894</v>
+        <v>45733</v>
       </c>
       <c r="EY4" s="92"/>
       <c r="EZ4" s="92"/>
@@ -2189,7 +2189,7 @@
       <c r="FD4" s="93"/>
       <c r="FE4" s="91">
         <f>FE5</f>
-        <v>45901</v>
+        <v>45740</v>
       </c>
       <c r="FF4" s="92"/>
       <c r="FG4" s="92"/>
@@ -2199,7 +2199,7 @@
       <c r="FK4" s="93"/>
       <c r="FL4" s="91">
         <f>FL5</f>
-        <v>45908</v>
+        <v>45747</v>
       </c>
       <c r="FM4" s="92"/>
       <c r="FN4" s="92"/>
@@ -2209,7 +2209,7 @@
       <c r="FR4" s="93"/>
       <c r="FS4" s="91">
         <f>FS5</f>
-        <v>45915</v>
+        <v>45754</v>
       </c>
       <c r="FT4" s="92"/>
       <c r="FU4" s="92"/>
@@ -2219,7 +2219,7 @@
       <c r="FY4" s="93"/>
       <c r="FZ4" s="91">
         <f>FZ5</f>
-        <v>45922</v>
+        <v>45761</v>
       </c>
       <c r="GA4" s="92"/>
       <c r="GB4" s="92"/>
@@ -2229,7 +2229,7 @@
       <c r="GF4" s="93"/>
       <c r="GG4" s="91">
         <f>GG5</f>
-        <v>45929</v>
+        <v>45768</v>
       </c>
       <c r="GH4" s="92"/>
       <c r="GI4" s="92"/>
@@ -2239,7 +2239,7 @@
       <c r="GM4" s="93"/>
       <c r="GN4" s="91">
         <f>GN5</f>
-        <v>45936</v>
+        <v>45775</v>
       </c>
       <c r="GO4" s="92"/>
       <c r="GP4" s="92"/>
@@ -2249,7 +2249,7 @@
       <c r="GT4" s="93"/>
       <c r="GU4" s="91">
         <f>GU5</f>
-        <v>45943</v>
+        <v>45782</v>
       </c>
       <c r="GV4" s="92"/>
       <c r="GW4" s="92"/>
@@ -2259,7 +2259,7 @@
       <c r="HA4" s="93"/>
       <c r="HB4" s="91">
         <f>HB5</f>
-        <v>45950</v>
+        <v>45789</v>
       </c>
       <c r="HC4" s="92"/>
       <c r="HD4" s="92"/>
@@ -2269,7 +2269,7 @@
       <c r="HH4" s="93"/>
       <c r="HI4" s="91">
         <f>HI5</f>
-        <v>45957</v>
+        <v>45796</v>
       </c>
       <c r="HJ4" s="92"/>
       <c r="HK4" s="92"/>
@@ -2279,7 +2279,7 @@
       <c r="HO4" s="93"/>
       <c r="HP4" s="91">
         <f>HP5</f>
-        <v>45964</v>
+        <v>45803</v>
       </c>
       <c r="HQ4" s="92"/>
       <c r="HR4" s="92"/>
@@ -2289,7 +2289,7 @@
       <c r="HV4" s="93"/>
       <c r="HW4" s="91">
         <f>HW5</f>
-        <v>45971</v>
+        <v>45810</v>
       </c>
       <c r="HX4" s="92"/>
       <c r="HY4" s="92"/>
@@ -2299,7 +2299,7 @@
       <c r="IC4" s="93"/>
       <c r="ID4" s="91">
         <f>ID5</f>
-        <v>45978</v>
+        <v>45817</v>
       </c>
       <c r="IE4" s="92"/>
       <c r="IF4" s="92"/>
@@ -2309,7 +2309,7 @@
       <c r="IJ4" s="93"/>
       <c r="IK4" s="91">
         <f>IK5</f>
-        <v>45985</v>
+        <v>45824</v>
       </c>
       <c r="IL4" s="92"/>
       <c r="IM4" s="92"/>
@@ -2319,7 +2319,7 @@
       <c r="IQ4" s="93"/>
       <c r="IR4" s="91">
         <f>IR5</f>
-        <v>45992</v>
+        <v>45831</v>
       </c>
       <c r="IS4" s="92"/>
       <c r="IT4" s="92"/>
@@ -2329,7 +2329,7 @@
       <c r="IX4" s="93"/>
       <c r="IY4" s="91">
         <f>IY5</f>
-        <v>45999</v>
+        <v>45838</v>
       </c>
       <c r="IZ4" s="92"/>
       <c r="JA4" s="92"/>
@@ -2339,7 +2339,7 @@
       <c r="JE4" s="93"/>
       <c r="JF4" s="91">
         <f>JF5</f>
-        <v>46006</v>
+        <v>45845</v>
       </c>
       <c r="JG4" s="92"/>
       <c r="JH4" s="92"/>
@@ -2349,7 +2349,7 @@
       <c r="JL4" s="93"/>
       <c r="JM4" s="91">
         <f>JM5</f>
-        <v>46013</v>
+        <v>45852</v>
       </c>
       <c r="JN4" s="92"/>
       <c r="JO4" s="92"/>
@@ -2368,1095 +2368,1095 @@
       <c r="E5" s="42"/>
       <c r="G5" s="58">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45747</v>
+        <v>45586</v>
       </c>
       <c r="H5" s="59">
         <f>G5+1</f>
-        <v>45748</v>
+        <v>45587</v>
       </c>
       <c r="I5" s="59">
         <f t="shared" ref="I5:AV5" si="0">H5+1</f>
-        <v>45749</v>
+        <v>45588</v>
       </c>
       <c r="J5" s="59">
         <f t="shared" si="0"/>
-        <v>45750</v>
+        <v>45589</v>
       </c>
       <c r="K5" s="59">
         <f t="shared" si="0"/>
-        <v>45751</v>
+        <v>45590</v>
       </c>
       <c r="L5" s="59">
         <f t="shared" si="0"/>
-        <v>45752</v>
+        <v>45591</v>
       </c>
       <c r="M5" s="60">
         <f t="shared" si="0"/>
-        <v>45753</v>
+        <v>45592</v>
       </c>
       <c r="N5" s="58">
         <f>M5+1</f>
-        <v>45754</v>
+        <v>45593</v>
       </c>
       <c r="O5" s="59">
         <f>N5+1</f>
-        <v>45755</v>
+        <v>45594</v>
       </c>
       <c r="P5" s="59">
         <f t="shared" si="0"/>
-        <v>45756</v>
+        <v>45595</v>
       </c>
       <c r="Q5" s="59">
         <f t="shared" si="0"/>
-        <v>45757</v>
+        <v>45596</v>
       </c>
       <c r="R5" s="59">
         <f t="shared" si="0"/>
-        <v>45758</v>
+        <v>45597</v>
       </c>
       <c r="S5" s="59">
         <f t="shared" si="0"/>
-        <v>45759</v>
+        <v>45598</v>
       </c>
       <c r="T5" s="60">
         <f t="shared" si="0"/>
-        <v>45760</v>
+        <v>45599</v>
       </c>
       <c r="U5" s="58">
         <f>T5+1</f>
-        <v>45761</v>
+        <v>45600</v>
       </c>
       <c r="V5" s="59">
         <f>U5+1</f>
-        <v>45762</v>
+        <v>45601</v>
       </c>
       <c r="W5" s="59">
         <f t="shared" si="0"/>
-        <v>45763</v>
+        <v>45602</v>
       </c>
       <c r="X5" s="59">
         <f t="shared" si="0"/>
-        <v>45764</v>
+        <v>45603</v>
       </c>
       <c r="Y5" s="59">
         <f t="shared" si="0"/>
-        <v>45765</v>
+        <v>45604</v>
       </c>
       <c r="Z5" s="59">
         <f t="shared" si="0"/>
-        <v>45766</v>
+        <v>45605</v>
       </c>
       <c r="AA5" s="60">
         <f t="shared" si="0"/>
-        <v>45767</v>
+        <v>45606</v>
       </c>
       <c r="AB5" s="58">
         <f>AA5+1</f>
-        <v>45768</v>
+        <v>45607</v>
       </c>
       <c r="AC5" s="59">
         <f>AB5+1</f>
-        <v>45769</v>
+        <v>45608</v>
       </c>
       <c r="AD5" s="59">
         <f t="shared" si="0"/>
-        <v>45770</v>
+        <v>45609</v>
       </c>
       <c r="AE5" s="59">
         <f t="shared" si="0"/>
-        <v>45771</v>
+        <v>45610</v>
       </c>
       <c r="AF5" s="59">
         <f t="shared" si="0"/>
-        <v>45772</v>
+        <v>45611</v>
       </c>
       <c r="AG5" s="59">
         <f t="shared" si="0"/>
-        <v>45773</v>
+        <v>45612</v>
       </c>
       <c r="AH5" s="60">
         <f t="shared" si="0"/>
-        <v>45774</v>
+        <v>45613</v>
       </c>
       <c r="AI5" s="58">
         <f>AH5+1</f>
-        <v>45775</v>
+        <v>45614</v>
       </c>
       <c r="AJ5" s="59">
         <f>AI5+1</f>
-        <v>45776</v>
+        <v>45615</v>
       </c>
       <c r="AK5" s="59">
         <f t="shared" si="0"/>
-        <v>45777</v>
+        <v>45616</v>
       </c>
       <c r="AL5" s="59">
         <f t="shared" si="0"/>
-        <v>45778</v>
+        <v>45617</v>
       </c>
       <c r="AM5" s="59">
         <f t="shared" si="0"/>
-        <v>45779</v>
+        <v>45618</v>
       </c>
       <c r="AN5" s="59">
         <f t="shared" si="0"/>
-        <v>45780</v>
+        <v>45619</v>
       </c>
       <c r="AO5" s="60">
         <f t="shared" si="0"/>
-        <v>45781</v>
+        <v>45620</v>
       </c>
       <c r="AP5" s="58">
         <f>AO5+1</f>
-        <v>45782</v>
+        <v>45621</v>
       </c>
       <c r="AQ5" s="59">
         <f>AP5+1</f>
-        <v>45783</v>
+        <v>45622</v>
       </c>
       <c r="AR5" s="59">
         <f t="shared" si="0"/>
-        <v>45784</v>
+        <v>45623</v>
       </c>
       <c r="AS5" s="59">
         <f t="shared" si="0"/>
-        <v>45785</v>
+        <v>45624</v>
       </c>
       <c r="AT5" s="59">
         <f t="shared" si="0"/>
-        <v>45786</v>
+        <v>45625</v>
       </c>
       <c r="AU5" s="59">
         <f t="shared" si="0"/>
-        <v>45787</v>
+        <v>45626</v>
       </c>
       <c r="AV5" s="60">
         <f t="shared" si="0"/>
-        <v>45788</v>
+        <v>45627</v>
       </c>
       <c r="AW5" s="58">
         <f>AV5+1</f>
-        <v>45789</v>
+        <v>45628</v>
       </c>
       <c r="AX5" s="59">
         <f>AW5+1</f>
-        <v>45790</v>
+        <v>45629</v>
       </c>
       <c r="AY5" s="59">
         <f t="shared" ref="AY5:BC5" si="1">AX5+1</f>
-        <v>45791</v>
+        <v>45630</v>
       </c>
       <c r="AZ5" s="59">
         <f t="shared" si="1"/>
-        <v>45792</v>
+        <v>45631</v>
       </c>
       <c r="BA5" s="59">
         <f t="shared" si="1"/>
-        <v>45793</v>
+        <v>45632</v>
       </c>
       <c r="BB5" s="59">
         <f t="shared" si="1"/>
-        <v>45794</v>
+        <v>45633</v>
       </c>
       <c r="BC5" s="60">
         <f t="shared" si="1"/>
-        <v>45795</v>
+        <v>45634</v>
       </c>
       <c r="BD5" s="58">
         <f>BC5+1</f>
-        <v>45796</v>
+        <v>45635</v>
       </c>
       <c r="BE5" s="59">
         <f>BD5+1</f>
-        <v>45797</v>
+        <v>45636</v>
       </c>
       <c r="BF5" s="59">
         <f t="shared" ref="BF5:BJ5" si="2">BE5+1</f>
-        <v>45798</v>
+        <v>45637</v>
       </c>
       <c r="BG5" s="59">
         <f t="shared" si="2"/>
-        <v>45799</v>
+        <v>45638</v>
       </c>
       <c r="BH5" s="59">
         <f t="shared" si="2"/>
-        <v>45800</v>
+        <v>45639</v>
       </c>
       <c r="BI5" s="59">
         <f t="shared" si="2"/>
-        <v>45801</v>
+        <v>45640</v>
       </c>
       <c r="BJ5" s="60">
         <f t="shared" si="2"/>
-        <v>45802</v>
+        <v>45641</v>
       </c>
       <c r="BK5" s="58">
         <f>BJ5+1</f>
-        <v>45803</v>
+        <v>45642</v>
       </c>
       <c r="BL5" s="59">
         <f>BK5+1</f>
-        <v>45804</v>
+        <v>45643</v>
       </c>
       <c r="BM5" s="59">
         <f t="shared" ref="BM5" si="3">BL5+1</f>
-        <v>45805</v>
+        <v>45644</v>
       </c>
       <c r="BN5" s="59">
         <f t="shared" ref="BN5" si="4">BM5+1</f>
-        <v>45806</v>
+        <v>45645</v>
       </c>
       <c r="BO5" s="59">
         <f t="shared" ref="BO5" si="5">BN5+1</f>
-        <v>45807</v>
+        <v>45646</v>
       </c>
       <c r="BP5" s="59">
         <f t="shared" ref="BP5" si="6">BO5+1</f>
-        <v>45808</v>
+        <v>45647</v>
       </c>
       <c r="BQ5" s="60">
         <f t="shared" ref="BQ5" si="7">BP5+1</f>
-        <v>45809</v>
+        <v>45648</v>
       </c>
       <c r="BR5" s="58">
         <f>BQ5+1</f>
-        <v>45810</v>
+        <v>45649</v>
       </c>
       <c r="BS5" s="59">
         <f>BR5+1</f>
-        <v>45811</v>
+        <v>45650</v>
       </c>
       <c r="BT5" s="59">
         <f t="shared" ref="BT5" si="8">BS5+1</f>
-        <v>45812</v>
+        <v>45651</v>
       </c>
       <c r="BU5" s="59">
         <f t="shared" ref="BU5" si="9">BT5+1</f>
-        <v>45813</v>
+        <v>45652</v>
       </c>
       <c r="BV5" s="59">
         <f t="shared" ref="BV5" si="10">BU5+1</f>
-        <v>45814</v>
+        <v>45653</v>
       </c>
       <c r="BW5" s="59">
         <f t="shared" ref="BW5" si="11">BV5+1</f>
-        <v>45815</v>
+        <v>45654</v>
       </c>
       <c r="BX5" s="60">
         <f t="shared" ref="BX5" si="12">BW5+1</f>
-        <v>45816</v>
+        <v>45655</v>
       </c>
       <c r="BY5" s="58">
         <f>BX5+1</f>
-        <v>45817</v>
+        <v>45656</v>
       </c>
       <c r="BZ5" s="59">
         <f>BY5+1</f>
-        <v>45818</v>
+        <v>45657</v>
       </c>
       <c r="CA5" s="59">
         <f t="shared" ref="CA5" si="13">BZ5+1</f>
-        <v>45819</v>
+        <v>45658</v>
       </c>
       <c r="CB5" s="59">
         <f t="shared" ref="CB5" si="14">CA5+1</f>
-        <v>45820</v>
+        <v>45659</v>
       </c>
       <c r="CC5" s="59">
         <f t="shared" ref="CC5" si="15">CB5+1</f>
-        <v>45821</v>
+        <v>45660</v>
       </c>
       <c r="CD5" s="59">
         <f t="shared" ref="CD5" si="16">CC5+1</f>
-        <v>45822</v>
+        <v>45661</v>
       </c>
       <c r="CE5" s="60">
         <f t="shared" ref="CE5" si="17">CD5+1</f>
-        <v>45823</v>
+        <v>45662</v>
       </c>
       <c r="CF5" s="58">
         <f>CE5+1</f>
-        <v>45824</v>
+        <v>45663</v>
       </c>
       <c r="CG5" s="59">
         <f>CF5+1</f>
-        <v>45825</v>
+        <v>45664</v>
       </c>
       <c r="CH5" s="59">
         <f t="shared" ref="CH5" si="18">CG5+1</f>
-        <v>45826</v>
+        <v>45665</v>
       </c>
       <c r="CI5" s="59">
         <f t="shared" ref="CI5" si="19">CH5+1</f>
-        <v>45827</v>
+        <v>45666</v>
       </c>
       <c r="CJ5" s="59">
         <f t="shared" ref="CJ5" si="20">CI5+1</f>
-        <v>45828</v>
+        <v>45667</v>
       </c>
       <c r="CK5" s="59">
         <f t="shared" ref="CK5" si="21">CJ5+1</f>
-        <v>45829</v>
+        <v>45668</v>
       </c>
       <c r="CL5" s="60">
         <f t="shared" ref="CL5" si="22">CK5+1</f>
-        <v>45830</v>
+        <v>45669</v>
       </c>
       <c r="CM5" s="58">
         <f>CL5+1</f>
-        <v>45831</v>
+        <v>45670</v>
       </c>
       <c r="CN5" s="59">
         <f>CM5+1</f>
-        <v>45832</v>
+        <v>45671</v>
       </c>
       <c r="CO5" s="59">
         <f t="shared" ref="CO5" si="23">CN5+1</f>
-        <v>45833</v>
+        <v>45672</v>
       </c>
       <c r="CP5" s="59">
         <f t="shared" ref="CP5" si="24">CO5+1</f>
-        <v>45834</v>
+        <v>45673</v>
       </c>
       <c r="CQ5" s="59">
         <f t="shared" ref="CQ5" si="25">CP5+1</f>
-        <v>45835</v>
+        <v>45674</v>
       </c>
       <c r="CR5" s="59">
         <f t="shared" ref="CR5" si="26">CQ5+1</f>
-        <v>45836</v>
+        <v>45675</v>
       </c>
       <c r="CS5" s="60">
         <f t="shared" ref="CS5" si="27">CR5+1</f>
-        <v>45837</v>
+        <v>45676</v>
       </c>
       <c r="CT5" s="58">
         <f>CS5+1</f>
-        <v>45838</v>
+        <v>45677</v>
       </c>
       <c r="CU5" s="59">
         <f>CT5+1</f>
-        <v>45839</v>
+        <v>45678</v>
       </c>
       <c r="CV5" s="59">
         <f t="shared" ref="CV5" si="28">CU5+1</f>
-        <v>45840</v>
+        <v>45679</v>
       </c>
       <c r="CW5" s="59">
         <f t="shared" ref="CW5" si="29">CV5+1</f>
-        <v>45841</v>
+        <v>45680</v>
       </c>
       <c r="CX5" s="59">
         <f t="shared" ref="CX5" si="30">CW5+1</f>
-        <v>45842</v>
+        <v>45681</v>
       </c>
       <c r="CY5" s="59">
         <f t="shared" ref="CY5" si="31">CX5+1</f>
-        <v>45843</v>
+        <v>45682</v>
       </c>
       <c r="CZ5" s="60">
         <f t="shared" ref="CZ5" si="32">CY5+1</f>
-        <v>45844</v>
+        <v>45683</v>
       </c>
       <c r="DA5" s="58">
         <f>CZ5+1</f>
-        <v>45845</v>
+        <v>45684</v>
       </c>
       <c r="DB5" s="59">
         <f>DA5+1</f>
-        <v>45846</v>
+        <v>45685</v>
       </c>
       <c r="DC5" s="59">
         <f t="shared" ref="DC5" si="33">DB5+1</f>
-        <v>45847</v>
+        <v>45686</v>
       </c>
       <c r="DD5" s="59">
         <f t="shared" ref="DD5" si="34">DC5+1</f>
-        <v>45848</v>
+        <v>45687</v>
       </c>
       <c r="DE5" s="59">
         <f t="shared" ref="DE5" si="35">DD5+1</f>
-        <v>45849</v>
+        <v>45688</v>
       </c>
       <c r="DF5" s="59">
         <f t="shared" ref="DF5" si="36">DE5+1</f>
-        <v>45850</v>
+        <v>45689</v>
       </c>
       <c r="DG5" s="60">
         <f t="shared" ref="DG5" si="37">DF5+1</f>
-        <v>45851</v>
+        <v>45690</v>
       </c>
       <c r="DH5" s="58">
         <f>DG5+1</f>
-        <v>45852</v>
+        <v>45691</v>
       </c>
       <c r="DI5" s="59">
         <f>DH5+1</f>
-        <v>45853</v>
+        <v>45692</v>
       </c>
       <c r="DJ5" s="59">
         <f t="shared" ref="DJ5" si="38">DI5+1</f>
-        <v>45854</v>
+        <v>45693</v>
       </c>
       <c r="DK5" s="59">
         <f t="shared" ref="DK5" si="39">DJ5+1</f>
-        <v>45855</v>
+        <v>45694</v>
       </c>
       <c r="DL5" s="59">
         <f t="shared" ref="DL5" si="40">DK5+1</f>
-        <v>45856</v>
+        <v>45695</v>
       </c>
       <c r="DM5" s="59">
         <f t="shared" ref="DM5" si="41">DL5+1</f>
-        <v>45857</v>
+        <v>45696</v>
       </c>
       <c r="DN5" s="60">
         <f t="shared" ref="DN5" si="42">DM5+1</f>
-        <v>45858</v>
+        <v>45697</v>
       </c>
       <c r="DO5" s="58">
         <f>DN5+1</f>
-        <v>45859</v>
+        <v>45698</v>
       </c>
       <c r="DP5" s="59">
         <f>DO5+1</f>
-        <v>45860</v>
+        <v>45699</v>
       </c>
       <c r="DQ5" s="59">
         <f t="shared" ref="DQ5" si="43">DP5+1</f>
-        <v>45861</v>
+        <v>45700</v>
       </c>
       <c r="DR5" s="59">
         <f t="shared" ref="DR5" si="44">DQ5+1</f>
-        <v>45862</v>
+        <v>45701</v>
       </c>
       <c r="DS5" s="59">
         <f t="shared" ref="DS5" si="45">DR5+1</f>
-        <v>45863</v>
+        <v>45702</v>
       </c>
       <c r="DT5" s="59">
         <f t="shared" ref="DT5" si="46">DS5+1</f>
-        <v>45864</v>
+        <v>45703</v>
       </c>
       <c r="DU5" s="60">
         <f t="shared" ref="DU5" si="47">DT5+1</f>
-        <v>45865</v>
+        <v>45704</v>
       </c>
       <c r="DV5" s="58">
         <f>DU5+1</f>
-        <v>45866</v>
+        <v>45705</v>
       </c>
       <c r="DW5" s="59">
         <f>DV5+1</f>
-        <v>45867</v>
+        <v>45706</v>
       </c>
       <c r="DX5" s="59">
         <f t="shared" ref="DX5" si="48">DW5+1</f>
-        <v>45868</v>
+        <v>45707</v>
       </c>
       <c r="DY5" s="59">
         <f t="shared" ref="DY5" si="49">DX5+1</f>
-        <v>45869</v>
+        <v>45708</v>
       </c>
       <c r="DZ5" s="59">
         <f t="shared" ref="DZ5" si="50">DY5+1</f>
-        <v>45870</v>
+        <v>45709</v>
       </c>
       <c r="EA5" s="59">
         <f t="shared" ref="EA5" si="51">DZ5+1</f>
-        <v>45871</v>
+        <v>45710</v>
       </c>
       <c r="EB5" s="60">
         <f t="shared" ref="EB5" si="52">EA5+1</f>
-        <v>45872</v>
+        <v>45711</v>
       </c>
       <c r="EC5" s="58">
         <f>EB5+1</f>
-        <v>45873</v>
+        <v>45712</v>
       </c>
       <c r="ED5" s="59">
         <f>EC5+1</f>
-        <v>45874</v>
+        <v>45713</v>
       </c>
       <c r="EE5" s="59">
         <f t="shared" ref="EE5" si="53">ED5+1</f>
-        <v>45875</v>
+        <v>45714</v>
       </c>
       <c r="EF5" s="59">
         <f t="shared" ref="EF5" si="54">EE5+1</f>
-        <v>45876</v>
+        <v>45715</v>
       </c>
       <c r="EG5" s="59">
         <f t="shared" ref="EG5" si="55">EF5+1</f>
-        <v>45877</v>
+        <v>45716</v>
       </c>
       <c r="EH5" s="59">
         <f t="shared" ref="EH5" si="56">EG5+1</f>
-        <v>45878</v>
+        <v>45717</v>
       </c>
       <c r="EI5" s="60">
         <f t="shared" ref="EI5" si="57">EH5+1</f>
-        <v>45879</v>
+        <v>45718</v>
       </c>
       <c r="EJ5" s="58">
         <f>EI5+1</f>
-        <v>45880</v>
+        <v>45719</v>
       </c>
       <c r="EK5" s="59">
         <f>EJ5+1</f>
-        <v>45881</v>
+        <v>45720</v>
       </c>
       <c r="EL5" s="59">
         <f t="shared" ref="EL5" si="58">EK5+1</f>
-        <v>45882</v>
+        <v>45721</v>
       </c>
       <c r="EM5" s="59">
         <f t="shared" ref="EM5" si="59">EL5+1</f>
-        <v>45883</v>
+        <v>45722</v>
       </c>
       <c r="EN5" s="59">
         <f t="shared" ref="EN5" si="60">EM5+1</f>
-        <v>45884</v>
+        <v>45723</v>
       </c>
       <c r="EO5" s="59">
         <f t="shared" ref="EO5" si="61">EN5+1</f>
-        <v>45885</v>
+        <v>45724</v>
       </c>
       <c r="EP5" s="60">
         <f t="shared" ref="EP5" si="62">EO5+1</f>
-        <v>45886</v>
+        <v>45725</v>
       </c>
       <c r="EQ5" s="58">
         <f>EP5+1</f>
-        <v>45887</v>
+        <v>45726</v>
       </c>
       <c r="ER5" s="59">
         <f>EQ5+1</f>
-        <v>45888</v>
+        <v>45727</v>
       </c>
       <c r="ES5" s="59">
         <f t="shared" ref="ES5" si="63">ER5+1</f>
-        <v>45889</v>
+        <v>45728</v>
       </c>
       <c r="ET5" s="59">
         <f t="shared" ref="ET5" si="64">ES5+1</f>
-        <v>45890</v>
+        <v>45729</v>
       </c>
       <c r="EU5" s="59">
         <f t="shared" ref="EU5" si="65">ET5+1</f>
-        <v>45891</v>
+        <v>45730</v>
       </c>
       <c r="EV5" s="59">
         <f t="shared" ref="EV5" si="66">EU5+1</f>
-        <v>45892</v>
+        <v>45731</v>
       </c>
       <c r="EW5" s="60">
         <f t="shared" ref="EW5" si="67">EV5+1</f>
-        <v>45893</v>
+        <v>45732</v>
       </c>
       <c r="EX5" s="58">
         <f>EW5+1</f>
-        <v>45894</v>
+        <v>45733</v>
       </c>
       <c r="EY5" s="59">
         <f>EX5+1</f>
-        <v>45895</v>
+        <v>45734</v>
       </c>
       <c r="EZ5" s="59">
         <f t="shared" ref="EZ5" si="68">EY5+1</f>
-        <v>45896</v>
+        <v>45735</v>
       </c>
       <c r="FA5" s="59">
         <f t="shared" ref="FA5" si="69">EZ5+1</f>
-        <v>45897</v>
+        <v>45736</v>
       </c>
       <c r="FB5" s="59">
         <f t="shared" ref="FB5" si="70">FA5+1</f>
-        <v>45898</v>
+        <v>45737</v>
       </c>
       <c r="FC5" s="59">
         <f t="shared" ref="FC5" si="71">FB5+1</f>
-        <v>45899</v>
+        <v>45738</v>
       </c>
       <c r="FD5" s="60">
         <f t="shared" ref="FD5" si="72">FC5+1</f>
-        <v>45900</v>
+        <v>45739</v>
       </c>
       <c r="FE5" s="58">
         <f>FD5+1</f>
-        <v>45901</v>
+        <v>45740</v>
       </c>
       <c r="FF5" s="59">
         <f>FE5+1</f>
-        <v>45902</v>
+        <v>45741</v>
       </c>
       <c r="FG5" s="59">
         <f t="shared" ref="FG5" si="73">FF5+1</f>
-        <v>45903</v>
+        <v>45742</v>
       </c>
       <c r="FH5" s="59">
         <f t="shared" ref="FH5" si="74">FG5+1</f>
-        <v>45904</v>
+        <v>45743</v>
       </c>
       <c r="FI5" s="59">
         <f t="shared" ref="FI5" si="75">FH5+1</f>
-        <v>45905</v>
+        <v>45744</v>
       </c>
       <c r="FJ5" s="59">
         <f t="shared" ref="FJ5" si="76">FI5+1</f>
-        <v>45906</v>
+        <v>45745</v>
       </c>
       <c r="FK5" s="60">
         <f t="shared" ref="FK5" si="77">FJ5+1</f>
-        <v>45907</v>
+        <v>45746</v>
       </c>
       <c r="FL5" s="58">
         <f>FK5+1</f>
-        <v>45908</v>
+        <v>45747</v>
       </c>
       <c r="FM5" s="59">
         <f>FL5+1</f>
-        <v>45909</v>
+        <v>45748</v>
       </c>
       <c r="FN5" s="59">
         <f t="shared" ref="FN5" si="78">FM5+1</f>
-        <v>45910</v>
+        <v>45749</v>
       </c>
       <c r="FO5" s="59">
         <f t="shared" ref="FO5" si="79">FN5+1</f>
-        <v>45911</v>
+        <v>45750</v>
       </c>
       <c r="FP5" s="59">
         <f t="shared" ref="FP5" si="80">FO5+1</f>
-        <v>45912</v>
+        <v>45751</v>
       </c>
       <c r="FQ5" s="59">
         <f t="shared" ref="FQ5" si="81">FP5+1</f>
-        <v>45913</v>
+        <v>45752</v>
       </c>
       <c r="FR5" s="60">
         <f t="shared" ref="FR5" si="82">FQ5+1</f>
-        <v>45914</v>
+        <v>45753</v>
       </c>
       <c r="FS5" s="58">
         <f>FR5+1</f>
-        <v>45915</v>
+        <v>45754</v>
       </c>
       <c r="FT5" s="59">
         <f>FS5+1</f>
-        <v>45916</v>
+        <v>45755</v>
       </c>
       <c r="FU5" s="59">
         <f t="shared" ref="FU5" si="83">FT5+1</f>
-        <v>45917</v>
+        <v>45756</v>
       </c>
       <c r="FV5" s="59">
         <f t="shared" ref="FV5" si="84">FU5+1</f>
-        <v>45918</v>
+        <v>45757</v>
       </c>
       <c r="FW5" s="59">
         <f t="shared" ref="FW5" si="85">FV5+1</f>
-        <v>45919</v>
+        <v>45758</v>
       </c>
       <c r="FX5" s="59">
         <f t="shared" ref="FX5" si="86">FW5+1</f>
-        <v>45920</v>
+        <v>45759</v>
       </c>
       <c r="FY5" s="60">
         <f t="shared" ref="FY5" si="87">FX5+1</f>
-        <v>45921</v>
+        <v>45760</v>
       </c>
       <c r="FZ5" s="58">
         <f>FY5+1</f>
-        <v>45922</v>
+        <v>45761</v>
       </c>
       <c r="GA5" s="59">
         <f>FZ5+1</f>
-        <v>45923</v>
+        <v>45762</v>
       </c>
       <c r="GB5" s="59">
         <f t="shared" ref="GB5" si="88">GA5+1</f>
-        <v>45924</v>
+        <v>45763</v>
       </c>
       <c r="GC5" s="59">
         <f t="shared" ref="GC5" si="89">GB5+1</f>
-        <v>45925</v>
+        <v>45764</v>
       </c>
       <c r="GD5" s="59">
         <f t="shared" ref="GD5" si="90">GC5+1</f>
-        <v>45926</v>
+        <v>45765</v>
       </c>
       <c r="GE5" s="59">
         <f t="shared" ref="GE5" si="91">GD5+1</f>
-        <v>45927</v>
+        <v>45766</v>
       </c>
       <c r="GF5" s="60">
         <f t="shared" ref="GF5" si="92">GE5+1</f>
-        <v>45928</v>
+        <v>45767</v>
       </c>
       <c r="GG5" s="58">
         <f>GF5+1</f>
-        <v>45929</v>
+        <v>45768</v>
       </c>
       <c r="GH5" s="59">
         <f>GG5+1</f>
-        <v>45930</v>
+        <v>45769</v>
       </c>
       <c r="GI5" s="59">
         <f t="shared" ref="GI5" si="93">GH5+1</f>
-        <v>45931</v>
+        <v>45770</v>
       </c>
       <c r="GJ5" s="59">
         <f t="shared" ref="GJ5" si="94">GI5+1</f>
-        <v>45932</v>
+        <v>45771</v>
       </c>
       <c r="GK5" s="59">
         <f t="shared" ref="GK5" si="95">GJ5+1</f>
-        <v>45933</v>
+        <v>45772</v>
       </c>
       <c r="GL5" s="59">
         <f t="shared" ref="GL5" si="96">GK5+1</f>
-        <v>45934</v>
+        <v>45773</v>
       </c>
       <c r="GM5" s="60">
         <f t="shared" ref="GM5" si="97">GL5+1</f>
-        <v>45935</v>
+        <v>45774</v>
       </c>
       <c r="GN5" s="58">
         <f>GM5+1</f>
-        <v>45936</v>
+        <v>45775</v>
       </c>
       <c r="GO5" s="59">
         <f>GN5+1</f>
-        <v>45937</v>
+        <v>45776</v>
       </c>
       <c r="GP5" s="59">
         <f t="shared" ref="GP5" si="98">GO5+1</f>
-        <v>45938</v>
+        <v>45777</v>
       </c>
       <c r="GQ5" s="59">
         <f t="shared" ref="GQ5" si="99">GP5+1</f>
-        <v>45939</v>
+        <v>45778</v>
       </c>
       <c r="GR5" s="59">
         <f t="shared" ref="GR5" si="100">GQ5+1</f>
-        <v>45940</v>
+        <v>45779</v>
       </c>
       <c r="GS5" s="59">
         <f t="shared" ref="GS5" si="101">GR5+1</f>
-        <v>45941</v>
+        <v>45780</v>
       </c>
       <c r="GT5" s="60">
         <f t="shared" ref="GT5" si="102">GS5+1</f>
-        <v>45942</v>
+        <v>45781</v>
       </c>
       <c r="GU5" s="58">
         <f>GT5+1</f>
-        <v>45943</v>
+        <v>45782</v>
       </c>
       <c r="GV5" s="59">
         <f>GU5+1</f>
-        <v>45944</v>
+        <v>45783</v>
       </c>
       <c r="GW5" s="59">
         <f t="shared" ref="GW5" si="103">GV5+1</f>
-        <v>45945</v>
+        <v>45784</v>
       </c>
       <c r="GX5" s="59">
         <f t="shared" ref="GX5" si="104">GW5+1</f>
-        <v>45946</v>
+        <v>45785</v>
       </c>
       <c r="GY5" s="59">
         <f t="shared" ref="GY5" si="105">GX5+1</f>
-        <v>45947</v>
+        <v>45786</v>
       </c>
       <c r="GZ5" s="59">
         <f t="shared" ref="GZ5" si="106">GY5+1</f>
-        <v>45948</v>
+        <v>45787</v>
       </c>
       <c r="HA5" s="60">
         <f t="shared" ref="HA5" si="107">GZ5+1</f>
-        <v>45949</v>
+        <v>45788</v>
       </c>
       <c r="HB5" s="58">
         <f>HA5+1</f>
-        <v>45950</v>
+        <v>45789</v>
       </c>
       <c r="HC5" s="59">
         <f>HB5+1</f>
-        <v>45951</v>
+        <v>45790</v>
       </c>
       <c r="HD5" s="59">
         <f t="shared" ref="HD5" si="108">HC5+1</f>
-        <v>45952</v>
+        <v>45791</v>
       </c>
       <c r="HE5" s="59">
         <f t="shared" ref="HE5" si="109">HD5+1</f>
-        <v>45953</v>
+        <v>45792</v>
       </c>
       <c r="HF5" s="59">
         <f t="shared" ref="HF5" si="110">HE5+1</f>
-        <v>45954</v>
+        <v>45793</v>
       </c>
       <c r="HG5" s="59">
         <f t="shared" ref="HG5" si="111">HF5+1</f>
-        <v>45955</v>
+        <v>45794</v>
       </c>
       <c r="HH5" s="60">
         <f t="shared" ref="HH5" si="112">HG5+1</f>
-        <v>45956</v>
+        <v>45795</v>
       </c>
       <c r="HI5" s="58">
         <f>HH5+1</f>
-        <v>45957</v>
+        <v>45796</v>
       </c>
       <c r="HJ5" s="59">
         <f>HI5+1</f>
-        <v>45958</v>
+        <v>45797</v>
       </c>
       <c r="HK5" s="59">
         <f t="shared" ref="HK5" si="113">HJ5+1</f>
-        <v>45959</v>
+        <v>45798</v>
       </c>
       <c r="HL5" s="59">
         <f t="shared" ref="HL5" si="114">HK5+1</f>
-        <v>45960</v>
+        <v>45799</v>
       </c>
       <c r="HM5" s="59">
         <f t="shared" ref="HM5" si="115">HL5+1</f>
-        <v>45961</v>
+        <v>45800</v>
       </c>
       <c r="HN5" s="59">
         <f t="shared" ref="HN5" si="116">HM5+1</f>
-        <v>45962</v>
+        <v>45801</v>
       </c>
       <c r="HO5" s="60">
         <f t="shared" ref="HO5" si="117">HN5+1</f>
-        <v>45963</v>
+        <v>45802</v>
       </c>
       <c r="HP5" s="58">
         <f>HO5+1</f>
-        <v>45964</v>
+        <v>45803</v>
       </c>
       <c r="HQ5" s="59">
         <f>HP5+1</f>
-        <v>45965</v>
+        <v>45804</v>
       </c>
       <c r="HR5" s="59">
         <f t="shared" ref="HR5" si="118">HQ5+1</f>
-        <v>45966</v>
+        <v>45805</v>
       </c>
       <c r="HS5" s="59">
         <f t="shared" ref="HS5" si="119">HR5+1</f>
-        <v>45967</v>
+        <v>45806</v>
       </c>
       <c r="HT5" s="59">
         <f t="shared" ref="HT5" si="120">HS5+1</f>
-        <v>45968</v>
+        <v>45807</v>
       </c>
       <c r="HU5" s="59">
         <f t="shared" ref="HU5" si="121">HT5+1</f>
-        <v>45969</v>
+        <v>45808</v>
       </c>
       <c r="HV5" s="60">
         <f t="shared" ref="HV5" si="122">HU5+1</f>
-        <v>45970</v>
+        <v>45809</v>
       </c>
       <c r="HW5" s="58">
         <f>HV5+1</f>
-        <v>45971</v>
+        <v>45810</v>
       </c>
       <c r="HX5" s="59">
         <f>HW5+1</f>
-        <v>45972</v>
+        <v>45811</v>
       </c>
       <c r="HY5" s="59">
         <f t="shared" ref="HY5" si="123">HX5+1</f>
-        <v>45973</v>
+        <v>45812</v>
       </c>
       <c r="HZ5" s="59">
         <f t="shared" ref="HZ5" si="124">HY5+1</f>
-        <v>45974</v>
+        <v>45813</v>
       </c>
       <c r="IA5" s="59">
         <f t="shared" ref="IA5" si="125">HZ5+1</f>
-        <v>45975</v>
+        <v>45814</v>
       </c>
       <c r="IB5" s="59">
         <f t="shared" ref="IB5" si="126">IA5+1</f>
-        <v>45976</v>
+        <v>45815</v>
       </c>
       <c r="IC5" s="60">
         <f t="shared" ref="IC5" si="127">IB5+1</f>
-        <v>45977</v>
+        <v>45816</v>
       </c>
       <c r="ID5" s="58">
         <f>IC5+1</f>
-        <v>45978</v>
+        <v>45817</v>
       </c>
       <c r="IE5" s="59">
         <f>ID5+1</f>
-        <v>45979</v>
+        <v>45818</v>
       </c>
       <c r="IF5" s="59">
         <f t="shared" ref="IF5" si="128">IE5+1</f>
-        <v>45980</v>
+        <v>45819</v>
       </c>
       <c r="IG5" s="59">
         <f t="shared" ref="IG5" si="129">IF5+1</f>
-        <v>45981</v>
+        <v>45820</v>
       </c>
       <c r="IH5" s="59">
         <f t="shared" ref="IH5" si="130">IG5+1</f>
-        <v>45982</v>
+        <v>45821</v>
       </c>
       <c r="II5" s="59">
         <f t="shared" ref="II5" si="131">IH5+1</f>
-        <v>45983</v>
+        <v>45822</v>
       </c>
       <c r="IJ5" s="60">
         <f t="shared" ref="IJ5" si="132">II5+1</f>
-        <v>45984</v>
+        <v>45823</v>
       </c>
       <c r="IK5" s="58">
         <f>IJ5+1</f>
-        <v>45985</v>
+        <v>45824</v>
       </c>
       <c r="IL5" s="59">
         <f>IK5+1</f>
-        <v>45986</v>
+        <v>45825</v>
       </c>
       <c r="IM5" s="59">
         <f t="shared" ref="IM5" si="133">IL5+1</f>
-        <v>45987</v>
+        <v>45826</v>
       </c>
       <c r="IN5" s="59">
         <f t="shared" ref="IN5" si="134">IM5+1</f>
-        <v>45988</v>
+        <v>45827</v>
       </c>
       <c r="IO5" s="59">
         <f t="shared" ref="IO5" si="135">IN5+1</f>
-        <v>45989</v>
+        <v>45828</v>
       </c>
       <c r="IP5" s="59">
         <f t="shared" ref="IP5" si="136">IO5+1</f>
-        <v>45990</v>
+        <v>45829</v>
       </c>
       <c r="IQ5" s="60">
         <f t="shared" ref="IQ5" si="137">IP5+1</f>
-        <v>45991</v>
+        <v>45830</v>
       </c>
       <c r="IR5" s="58">
         <f>IQ5+1</f>
-        <v>45992</v>
+        <v>45831</v>
       </c>
       <c r="IS5" s="59">
         <f>IR5+1</f>
-        <v>45993</v>
+        <v>45832</v>
       </c>
       <c r="IT5" s="59">
         <f t="shared" ref="IT5" si="138">IS5+1</f>
-        <v>45994</v>
+        <v>45833</v>
       </c>
       <c r="IU5" s="59">
         <f t="shared" ref="IU5" si="139">IT5+1</f>
-        <v>45995</v>
+        <v>45834</v>
       </c>
       <c r="IV5" s="59">
         <f t="shared" ref="IV5" si="140">IU5+1</f>
-        <v>45996</v>
+        <v>45835</v>
       </c>
       <c r="IW5" s="59">
         <f t="shared" ref="IW5" si="141">IV5+1</f>
-        <v>45997</v>
+        <v>45836</v>
       </c>
       <c r="IX5" s="60">
         <f t="shared" ref="IX5" si="142">IW5+1</f>
-        <v>45998</v>
+        <v>45837</v>
       </c>
       <c r="IY5" s="58">
         <f>IX5+1</f>
-        <v>45999</v>
+        <v>45838</v>
       </c>
       <c r="IZ5" s="59">
         <f>IY5+1</f>
-        <v>46000</v>
+        <v>45839</v>
       </c>
       <c r="JA5" s="59">
         <f t="shared" ref="JA5" si="143">IZ5+1</f>
-        <v>46001</v>
+        <v>45840</v>
       </c>
       <c r="JB5" s="59">
         <f t="shared" ref="JB5" si="144">JA5+1</f>
-        <v>46002</v>
+        <v>45841</v>
       </c>
       <c r="JC5" s="59">
         <f t="shared" ref="JC5" si="145">JB5+1</f>
-        <v>46003</v>
+        <v>45842</v>
       </c>
       <c r="JD5" s="59">
         <f t="shared" ref="JD5" si="146">JC5+1</f>
-        <v>46004</v>
+        <v>45843</v>
       </c>
       <c r="JE5" s="60">
         <f t="shared" ref="JE5" si="147">JD5+1</f>
-        <v>46005</v>
+        <v>45844</v>
       </c>
       <c r="JF5" s="58">
         <f>JE5+1</f>
-        <v>46006</v>
+        <v>45845</v>
       </c>
       <c r="JG5" s="59">
         <f>JF5+1</f>
-        <v>46007</v>
+        <v>45846</v>
       </c>
       <c r="JH5" s="59">
         <f t="shared" ref="JH5" si="148">JG5+1</f>
-        <v>46008</v>
+        <v>45847</v>
       </c>
       <c r="JI5" s="59">
         <f t="shared" ref="JI5" si="149">JH5+1</f>
-        <v>46009</v>
+        <v>45848</v>
       </c>
       <c r="JJ5" s="59">
         <f t="shared" ref="JJ5" si="150">JI5+1</f>
-        <v>46010</v>
+        <v>45849</v>
       </c>
       <c r="JK5" s="59">
         <f t="shared" ref="JK5" si="151">JJ5+1</f>
-        <v>46011</v>
+        <v>45850</v>
       </c>
       <c r="JL5" s="60">
         <f t="shared" ref="JL5" si="152">JK5+1</f>
-        <v>46012</v>
+        <v>45851</v>
       </c>
       <c r="JM5" s="58">
         <f>JL5+1</f>
-        <v>46013</v>
+        <v>45852</v>
       </c>
       <c r="JN5" s="59">
         <f>JM5+1</f>
-        <v>46014</v>
+        <v>45853</v>
       </c>
       <c r="JO5" s="59">
         <f t="shared" ref="JO5" si="153">JN5+1</f>
-        <v>46015</v>
+        <v>45854</v>
       </c>
       <c r="JP5" s="59">
         <f t="shared" ref="JP5" si="154">JO5+1</f>
-        <v>46016</v>
+        <v>45855</v>
       </c>
       <c r="JQ5" s="59">
         <f t="shared" ref="JQ5" si="155">JP5+1</f>
-        <v>46017</v>
+        <v>45856</v>
       </c>
       <c r="JR5" s="59">
         <f t="shared" ref="JR5" si="156">JQ5+1</f>
-        <v>46018</v>
+        <v>45857</v>
       </c>
       <c r="JS5" s="60">
         <f t="shared" ref="JS5" si="157">JR5+1</f>
-        <v>46019</v>
+        <v>45858</v>
       </c>
     </row>
     <row r="6" spans="1:279" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8998,7 +8998,7 @@
       </c>
       <c r="C22" s="72">
         <f t="shared" ref="C22" si="170">SUM(C23:C24)/COUNT(C23:C24)</f>
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="D22" s="73">
         <f t="shared" si="169"/>
@@ -9292,7 +9292,7 @@
         <v>58</v>
       </c>
       <c r="C23" s="75">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="D23" s="76">
         <f t="shared" ref="D23" si="171">D22</f>
@@ -11646,6 +11646,37 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="JM4:JS4"/>
+    <mergeCell ref="ID4:IJ4"/>
+    <mergeCell ref="IK4:IQ4"/>
+    <mergeCell ref="IR4:IX4"/>
+    <mergeCell ref="IY4:JE4"/>
+    <mergeCell ref="JF4:JL4"/>
+    <mergeCell ref="GU4:HA4"/>
+    <mergeCell ref="HB4:HH4"/>
+    <mergeCell ref="HI4:HO4"/>
+    <mergeCell ref="HP4:HV4"/>
+    <mergeCell ref="HW4:IC4"/>
+    <mergeCell ref="FL4:FR4"/>
+    <mergeCell ref="FS4:FY4"/>
+    <mergeCell ref="FZ4:GF4"/>
+    <mergeCell ref="GG4:GM4"/>
+    <mergeCell ref="GN4:GT4"/>
+    <mergeCell ref="EC4:EI4"/>
+    <mergeCell ref="EJ4:EP4"/>
+    <mergeCell ref="EQ4:EW4"/>
+    <mergeCell ref="EX4:FD4"/>
+    <mergeCell ref="FE4:FK4"/>
+    <mergeCell ref="CT4:CZ4"/>
+    <mergeCell ref="DA4:DG4"/>
+    <mergeCell ref="DH4:DN4"/>
+    <mergeCell ref="DO4:DU4"/>
+    <mergeCell ref="DV4:EB4"/>
+    <mergeCell ref="BK4:BQ4"/>
+    <mergeCell ref="BR4:BX4"/>
+    <mergeCell ref="BY4:CE4"/>
+    <mergeCell ref="CF4:CL4"/>
+    <mergeCell ref="CM4:CS4"/>
     <mergeCell ref="AI4:AO4"/>
     <mergeCell ref="AP4:AV4"/>
     <mergeCell ref="AW4:BC4"/>
@@ -11655,37 +11686,6 @@
     <mergeCell ref="N4:T4"/>
     <mergeCell ref="U4:AA4"/>
     <mergeCell ref="AB4:AH4"/>
-    <mergeCell ref="BK4:BQ4"/>
-    <mergeCell ref="BR4:BX4"/>
-    <mergeCell ref="BY4:CE4"/>
-    <mergeCell ref="CF4:CL4"/>
-    <mergeCell ref="CM4:CS4"/>
-    <mergeCell ref="CT4:CZ4"/>
-    <mergeCell ref="DA4:DG4"/>
-    <mergeCell ref="DH4:DN4"/>
-    <mergeCell ref="DO4:DU4"/>
-    <mergeCell ref="DV4:EB4"/>
-    <mergeCell ref="EC4:EI4"/>
-    <mergeCell ref="EJ4:EP4"/>
-    <mergeCell ref="EQ4:EW4"/>
-    <mergeCell ref="EX4:FD4"/>
-    <mergeCell ref="FE4:FK4"/>
-    <mergeCell ref="FL4:FR4"/>
-    <mergeCell ref="FS4:FY4"/>
-    <mergeCell ref="FZ4:GF4"/>
-    <mergeCell ref="GG4:GM4"/>
-    <mergeCell ref="GN4:GT4"/>
-    <mergeCell ref="GU4:HA4"/>
-    <mergeCell ref="HB4:HH4"/>
-    <mergeCell ref="HI4:HO4"/>
-    <mergeCell ref="HP4:HV4"/>
-    <mergeCell ref="HW4:IC4"/>
-    <mergeCell ref="JM4:JS4"/>
-    <mergeCell ref="ID4:IJ4"/>
-    <mergeCell ref="IK4:IQ4"/>
-    <mergeCell ref="IR4:IX4"/>
-    <mergeCell ref="IY4:JE4"/>
-    <mergeCell ref="JF4:JL4"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
   <conditionalFormatting sqref="C7:C30">
@@ -11722,7 +11722,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="10" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -11854,23 +11854,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12162,22 +12151,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12204,9 +12200,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>